<commit_message>
dodanie ekipy od TZI do zestawienia
</commit_message>
<xml_diff>
--- a/plan/Ekipy budowlane.xlsx
+++ b/plan/Ekipy budowlane.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="Oferty" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="154">
   <si>
     <t>Dotychczasowe realizacje</t>
   </si>
@@ -223,27 +223,9 @@
     <t xml:space="preserve">nie  </t>
   </si>
   <si>
-    <t>nie mają kierownika budowy, osobą odpowiedzialną za kontak jest Nowak</t>
-  </si>
-  <si>
     <t>tak</t>
   </si>
   <si>
-    <t>ogrodzenie działki po stronie inwestora</t>
-  </si>
-  <si>
-    <t>nie ma problemu, sugeruje, ze drobne zmiany w ramach pierwotnej wyceny</t>
-  </si>
-  <si>
-    <t>ma agregat, woda jest zamawiana</t>
-  </si>
-  <si>
-    <t>dostarczył</t>
-  </si>
-  <si>
-    <t>rozliczenie po etapach</t>
-  </si>
-  <si>
     <t>Ogólne wrażenie</t>
   </si>
   <si>
@@ -259,192 +241,245 @@
     <t>buduje raczej z ceramiki</t>
   </si>
   <si>
-    <t>ma zasadę aneksów do projektu, nie widzi przeszkód w zmianie otworów okiennych</t>
-  </si>
-  <si>
-    <t>nie sugeruje sam, robi to co inwestor chce
-poleca kostę brukową</t>
-  </si>
-  <si>
-    <t>poleca kostkę brukową</t>
-  </si>
-  <si>
-    <t>nie wygląda na speca od płyt fundamentowych, 
-sugeruje, ze WG jest niezbędna przy kominku
+    <t>ok..5 miesięcy (niestety nie pamiętam czy z dachem, którego nie robi, czy bez dachu)</t>
+  </si>
+  <si>
+    <t>TZI-Team</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Lp</t>
+  </si>
+  <si>
+    <t>Etapy robót budowlanych</t>
+  </si>
+  <si>
+    <t>Robocizna netto</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>Usunięcie  humusu  fadromą</t>
+  </si>
+  <si>
+    <t>Ława – wykop</t>
+  </si>
+  <si>
+    <t>Podkład z betonu</t>
+  </si>
+  <si>
+    <t>Szalowanie – przygotowanie i montaż zbrojenia</t>
+  </si>
+  <si>
+    <t>Ułożenie betonu</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>Fundament</t>
+  </si>
+  <si>
+    <t>Izolacja pozioma</t>
+  </si>
+  <si>
+    <t>Mur z bloczków betonowych</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>Izolacja fundamentu</t>
+  </si>
+  <si>
+    <t>Zasypanie piaskiem</t>
+  </si>
+  <si>
+    <t>Zagęszczenie zagęszczarką</t>
+  </si>
+  <si>
+    <t>Ułożenie kanalizacji</t>
+  </si>
+  <si>
+    <t>Płyta betonowa</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>Parter</t>
+  </si>
+  <si>
+    <t>Mur parteru</t>
+  </si>
+  <si>
+    <t>Komin</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>Strop</t>
+  </si>
+  <si>
+    <t>Przygotowanie zbrojenia podciągów i wieńca ,schody</t>
+  </si>
+  <si>
+    <t>Wylanie betonu</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>Ściana kolankowa</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>Mur poddasza</t>
+  </si>
+  <si>
+    <t>Szczyty</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>Konstrukcja więżby</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>Pokrycie dachu</t>
+  </si>
+  <si>
+    <t>Folia</t>
+  </si>
+  <si>
+    <t>Okna</t>
+  </si>
+  <si>
+    <t>Obróbki blacharskie</t>
+  </si>
+  <si>
+    <t>Orynnowanie</t>
+  </si>
+  <si>
+    <t>Sprzęt oraz deskowanie ( szalunki , stemple ) po stronie Wykonawcy .</t>
+  </si>
+  <si>
+    <t>Razem</t>
+  </si>
+  <si>
+    <t>Wieniec, trzpienie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Komin                              </t>
+  </si>
+  <si>
+    <t>Kontrłata, łata</t>
+  </si>
+  <si>
+    <t>Robocizna brutto</t>
+  </si>
+  <si>
+    <t>Docieplenie fundamentu styropianem</t>
+  </si>
+  <si>
+    <t>http://www.domyosolin.pl, telefony na byłych inwestorów na życzenie</t>
+  </si>
+  <si>
+    <t>Zakup i dostawa materiałów jest po stronie wykonawcy</t>
+  </si>
+  <si>
+    <t>Preferuje ceramikę, ale budował z betonu (jakiś kościół)</t>
+  </si>
+  <si>
+    <t>Marek, TZI</t>
+  </si>
+  <si>
+    <t>Z tego co się zorientowałam ma własnych pracowników, w tym TZI-ego od marca</t>
+  </si>
+  <si>
+    <t>Nie posiadają agregatu, prąd powinien być na działce. Woda z hydrantu.</t>
+  </si>
+  <si>
+    <t>Nie ma problemu, sugeruje, ze drobne zmiany w ramach pierwotnej wyceny</t>
+  </si>
+  <si>
+    <t>Ma agregat, wodę sugeruje pobierać z hydrantu.</t>
+  </si>
+  <si>
+    <t>Ma zasadę aneksów do projektu, nie widzi przeszkód w zmianie otworów okiennych</t>
+  </si>
+  <si>
+    <t>Poleca kostkę brukową</t>
+  </si>
+  <si>
+    <t>Nie sugeruje sam, robi to co inwestor chce. Poleca kostę brukową</t>
+  </si>
+  <si>
+    <t>Wygląda na godnego zaufania, ma dobrą motywację do tej roboty</t>
+  </si>
+  <si>
+    <t>Nie wygląda na speca od płyt fundamentowych. Sugeruje, ze WG jest niezbędna przy kominku
 nie robi dachu</t>
   </si>
   <si>
-    <t>nie robi dachu</t>
-  </si>
-  <si>
-    <t>ma agregat, wodę sugeruje pobierać z hydrantu</t>
-  </si>
-  <si>
-    <t>zdjęcie humusu - inwestor
- - geodeta - inwestor
-pozostałe - wykonawca</t>
-  </si>
-  <si>
-    <t>ok..5 miesięcy (niestety nie pamiętam czy z dachem, którego nie robi, czy bez dachu)</t>
-  </si>
-  <si>
-    <t>TZI-Team</t>
-  </si>
-  <si>
-    <t>wygląda na godnego zaufania, ma dobrą motywację do tej roboty</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Lp</t>
-  </si>
-  <si>
-    <t>Etapy robót budowlanych</t>
-  </si>
-  <si>
-    <t>Robocizna netto</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>Usunięcie  humusu  fadromą</t>
-  </si>
-  <si>
-    <t>Ława – wykop</t>
-  </si>
-  <si>
-    <t>Podkład z betonu</t>
-  </si>
-  <si>
-    <t>Szalowanie – przygotowanie i montaż zbrojenia</t>
-  </si>
-  <si>
-    <t>Ułożenie betonu</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>Fundament</t>
-  </si>
-  <si>
-    <t>Izolacja pozioma</t>
-  </si>
-  <si>
-    <t>Mur z bloczków betonowych</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>Izolacja fundamentu</t>
-  </si>
-  <si>
-    <t>Zasypanie piaskiem</t>
-  </si>
-  <si>
-    <t>Zagęszczenie zagęszczarką</t>
-  </si>
-  <si>
-    <t>Ułożenie kanalizacji</t>
-  </si>
-  <si>
-    <t>Płyta betonowa</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>Parter</t>
-  </si>
-  <si>
-    <t>Mur parteru</t>
-  </si>
-  <si>
-    <t>Komin</t>
-  </si>
-  <si>
-    <t>6.</t>
-  </si>
-  <si>
-    <t>Strop</t>
-  </si>
-  <si>
-    <t>Przygotowanie zbrojenia podciągów i wieńca ,schody</t>
-  </si>
-  <si>
-    <t>Wylanie betonu</t>
-  </si>
-  <si>
-    <t>7.</t>
-  </si>
-  <si>
-    <t>Ściana kolankowa</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>Mur poddasza</t>
-  </si>
-  <si>
-    <t>Szczyty</t>
-  </si>
-  <si>
-    <t>9.</t>
-  </si>
-  <si>
-    <t>Konstrukcja więżby</t>
-  </si>
-  <si>
-    <t>10.</t>
-  </si>
-  <si>
-    <t>Pokrycie dachu</t>
-  </si>
-  <si>
-    <t>Folia</t>
-  </si>
-  <si>
-    <t>Okna</t>
-  </si>
-  <si>
-    <t>Obróbki blacharskie</t>
-  </si>
-  <si>
-    <t>Orynnowanie</t>
-  </si>
-  <si>
-    <t>Sprzęt oraz deskowanie ( szalunki , stemple ) po stronie Wykonawcy .</t>
-  </si>
-  <si>
-    <t>Razem</t>
-  </si>
-  <si>
-    <t>Wieniec, trzpienie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Komin                              </t>
-  </si>
-  <si>
-    <t>Kontrłata, łata</t>
-  </si>
-  <si>
-    <t>Robocizna brutto</t>
-  </si>
-  <si>
-    <t>Docieplenie fundamentu styropianem</t>
+    <t>Nie robi dachu</t>
+  </si>
+  <si>
+    <t>Zdjęcie humusu - inwestor, Geodeta - inwestor, Pozostałe - wykonawca</t>
+  </si>
+  <si>
+    <t>Ogrodzenie działki po stronie inwestora</t>
+  </si>
+  <si>
+    <t>Ogrodzenie działki po stronie Inwestora (możliwe przerzucenie na wykonawcę). Maja własne toalety, magazynki na materiały.</t>
+  </si>
+  <si>
+    <t>Raczej nie ma problemu. Pod warunkim zatwierdzenia zmian przez kierownika budowy (usunięcie komina). Zmiany w formie aneksu (dopisanie pozycji). Zrobią słupki w otworach okiennych.</t>
+  </si>
+  <si>
+    <t>Zadeklarował, że będzie proponował lepsze rozwiązania jeśli takie zna. Od razu zaproponował podniesienie ścianki kolankowej. Zaproponował spadek dachu lukarny, schody drewniane, kosmetykę dachu.</t>
+  </si>
+  <si>
+    <t>Robi do stanu deweloperskiego.</t>
+  </si>
+  <si>
+    <t>Jest zaliczka. Rozliczenie po zakończeniu etapu. Wycena zawiera wszystko (ceny materiałów zawierają 15% zniżki w hurtowni, pozostałe 5%zniżki wykonawca traktuje sobie jako koszt zakupu materiału). Faktury z 8% Vatem. Stawki nie ulegają zmianie.</t>
+  </si>
+  <si>
+    <t>Rozliczenie po etapach</t>
+  </si>
+  <si>
+    <t>Dostarczył</t>
+  </si>
+  <si>
+    <t>Ma agregat, woda jest zamawiana</t>
+  </si>
+  <si>
+    <t>Nie mają kierownika budowy, osobą odpowiedzialną za kontak jest Nowak</t>
+  </si>
+  <si>
+    <t>Nie mają kierownika budowy. Pozytywnie nastawieni na KB Inwestora. Wykonuja dokumentację zdjęciową etapów.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-8 tygodni SSZ (bez okien). </t>
   </si>
 </sst>
 </file>
@@ -793,8 +828,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -803,119 +836,121 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1495,16 +1530,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
   </cols>
@@ -1514,16 +1550,16 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1543,7 +1579,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" ht="21">
+    <row r="3" spans="1:7" ht="22.5">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
@@ -1554,11 +1590,13 @@
         <v>61</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="64.5">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1566,10 +1604,12 @@
         <v>62</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="12" t="s">
+        <v>127</v>
+      </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
     </row>
@@ -1580,7 +1620,7 @@
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
@@ -1591,7 +1631,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
@@ -1603,14 +1643,16 @@
         <v>63</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12" t="s">
+        <v>153</v>
+      </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" ht="22.5">
+    <row r="8" spans="1:7" ht="54">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -1618,14 +1660,16 @@
         <v>64</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="31.5">
+    <row r="9" spans="1:7" ht="54">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -1633,25 +1677,29 @@
         <v>65</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="12" t="s">
+        <v>129</v>
+      </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="42">
+    <row r="10" spans="1:7" ht="127.5">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="12" t="s">
+        <v>145</v>
+      </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
     </row>
@@ -1662,7 +1710,7 @@
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
@@ -1671,17 +1719,19 @@
         <v>47</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7" ht="21">
+    <row r="13" spans="1:7" ht="64.5">
       <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1740,9 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="12" t="s">
+        <v>131</v>
+      </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
@@ -1702,23 +1754,27 @@
         <v>67</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="12" t="s">
+        <v>146</v>
+      </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="31.5">
+    <row r="15" spans="1:7" ht="85.5">
       <c r="A15" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="12" t="s">
+        <v>152</v>
+      </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
@@ -1727,56 +1783,64 @@
         <v>6</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" ht="43.5">
+    <row r="17" spans="1:7" ht="85.5">
       <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" ht="52.5">
+    <row r="18" spans="1:7" ht="127.5">
       <c r="A18" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" ht="33">
+    <row r="19" spans="1:7" ht="54">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
     </row>
@@ -1785,7 +1849,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1793,16 +1857,18 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="159">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="13" t="s">
+        <v>147</v>
+      </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
@@ -1841,13 +1907,13 @@
     </row>
     <row r="25" spans="1:7" ht="64.5">
       <c r="A25" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
@@ -1856,7 +1922,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -2131,11 +2197,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
@@ -2459,7 +2525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2472,339 +2538,334 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
+      <c r="A2" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="62"/>
+      <c r="B3" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
+      <c r="A4" s="62"/>
+      <c r="B4" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+    </row>
+    <row r="5" spans="1:4" ht="31.5">
+      <c r="A5" s="62"/>
+      <c r="B5" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A6" s="63"/>
+      <c r="B6" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75">
+      <c r="A8" s="62"/>
+      <c r="B8" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A9" s="63"/>
+      <c r="B9" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75">
+      <c r="A10" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75">
+      <c r="A11" s="62"/>
+      <c r="B11" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75">
+      <c r="A12" s="62"/>
+      <c r="B12" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="51" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="43" t="s">
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75">
+      <c r="A13" s="62"/>
+      <c r="B13" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A14" s="63"/>
+      <c r="B14" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A15" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46" t="s">
+      <c r="B15" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75">
+      <c r="A16" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46" t="s">
+      <c r="B16" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75">
+      <c r="A17" s="59"/>
+      <c r="B17" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
+      <c r="A18" s="59"/>
+      <c r="B18" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
-      <c r="A7" s="43" t="s">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A19" s="60"/>
+      <c r="B19" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75">
+      <c r="A20" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75">
-      <c r="A8" s="45"/>
-      <c r="B8" s="47" t="s">
+      <c r="B20" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50" t="s">
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+    </row>
+    <row r="21" spans="1:4" ht="31.5">
+      <c r="A21" s="59"/>
+      <c r="B21" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75">
-      <c r="A10" s="43" t="s">
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A22" s="59"/>
+      <c r="B22" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
+      <c r="A23" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75">
-      <c r="A11" s="45"/>
-      <c r="B11" s="47" t="s">
+      <c r="B23" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75">
-      <c r="A12" s="45"/>
-      <c r="B12" s="47" t="s">
+      <c r="C23" s="50"/>
+      <c r="D23" s="52"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A24" s="56"/>
+      <c r="B24" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="51"/>
+      <c r="D24" s="53"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75">
+      <c r="A25" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75">
-      <c r="A13" s="45"/>
-      <c r="B13" s="47" t="s">
+      <c r="B25" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A14" s="48"/>
-      <c r="B14" s="50" t="s">
+      <c r="C25" s="52"/>
+      <c r="D25" s="55"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75">
+      <c r="A26" s="55"/>
+      <c r="B26" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-    </row>
-    <row r="15" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A15" s="49" t="s">
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A27" s="56"/>
+      <c r="B27" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="53"/>
+      <c r="D27" s="56"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75">
+      <c r="A28" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75">
-      <c r="A16" s="26" t="s">
+      <c r="B28" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A29" s="49"/>
+      <c r="B29" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75">
+      <c r="A30" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29" t="s">
+      <c r="B30" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-    </row>
-    <row r="19" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31" t="s">
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75">
+      <c r="A31" s="48"/>
+      <c r="B31" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75">
-      <c r="A20" s="28" t="s">
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="48"/>
+      <c r="B32" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75">
+      <c r="A33" s="48"/>
+      <c r="B33" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75">
+      <c r="A34" s="48"/>
+      <c r="B34" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29" t="s">
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+    </row>
+    <row r="35" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A35" s="49"/>
+      <c r="B35" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-    </row>
-    <row r="22" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29" t="s">
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+    </row>
+    <row r="36" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A36" s="22"/>
+      <c r="B36" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75">
+      <c r="A37" s="21"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75">
-      <c r="A23" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="54"/>
-    </row>
-    <row r="24" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="55"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75">
-      <c r="A25" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="36"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="36"/>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="34"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75">
-      <c r="A28" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-    </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75">
-      <c r="A30" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75">
-      <c r="A31" s="39"/>
-      <c r="B31" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-    </row>
-    <row r="35" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A35" s="41"/>
-      <c r="B35" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-    </row>
-    <row r="36" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75">
-      <c r="A37" s="23"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="25" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A2:A6"/>
     <mergeCell ref="A30:A35"/>
     <mergeCell ref="C30:C35"/>
     <mergeCell ref="D30:D35"/>
@@ -2817,11 +2878,16 @@
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
wybranie ekipy, kosztorys dla banku
</commit_message>
<xml_diff>
--- a/plan/Ekipy budowlane.xlsx
+++ b/plan/Ekipy budowlane.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Oferty" sheetId="1" r:id="rId1"/>
     <sheet name="Szablon oferty" sheetId="3" r:id="rId2"/>
     <sheet name="Kosztorys - szablon" sheetId="2" r:id="rId3"/>
     <sheet name="Kosztorysy ekip - zestawienie" sheetId="4" r:id="rId4"/>
+    <sheet name="Kosztorys" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="194">
   <si>
     <t>Dotychczasowe realizacje</t>
   </si>
@@ -450,13 +451,166 @@
   </si>
   <si>
     <t>TZI - inwestor</t>
+  </si>
+  <si>
+    <t>TZI</t>
+  </si>
+  <si>
+    <t>płyta</t>
+  </si>
+  <si>
+    <t>funadament</t>
+  </si>
+  <si>
+    <t>ściany nośne</t>
+  </si>
+  <si>
+    <t>strop (bez pompy)</t>
+  </si>
+  <si>
+    <t>komin</t>
+  </si>
+  <si>
+    <t>ścianki działowe</t>
+  </si>
+  <si>
+    <t>dach (Nowak)</t>
+  </si>
+  <si>
+    <t>zbrojenie</t>
+  </si>
+  <si>
+    <t>materiał netto</t>
+  </si>
+  <si>
+    <t>materał S</t>
+  </si>
+  <si>
+    <t>materiał TZI</t>
+  </si>
+  <si>
+    <t>suma</t>
+  </si>
+  <si>
+    <t>1 Roboty ziemne</t>
+  </si>
+  <si>
+    <t>2 Fundamenty, izolacje</t>
+  </si>
+  <si>
+    <t>3 Sciany i stropy piwnic</t>
+  </si>
+  <si>
+    <t>I STAN ZEROWY RAZEM</t>
+  </si>
+  <si>
+    <t>4 Sciany nosne, kominy,</t>
+  </si>
+  <si>
+    <t>5 Stropy, schody</t>
+  </si>
+  <si>
+    <t>6 Konstrukcja dachu</t>
+  </si>
+  <si>
+    <t>7 Pokrycie, obróbki dachu</t>
+  </si>
+  <si>
+    <t>8 Stolarka zewnetrzna</t>
+  </si>
+  <si>
+    <t>9 Sciany działowe</t>
+  </si>
+  <si>
+    <t>10 Wylewki cementowe (szlichta</t>
+  </si>
+  <si>
+    <t>11 Izolacja termiczna dachu</t>
+  </si>
+  <si>
+    <t>12a Instalacje wewnetrzne- wod-kan</t>
+  </si>
+  <si>
+    <t>12d Instalacje wewnetrzne-c.o.</t>
+  </si>
+  <si>
+    <t>12e Instalacje wewnetrzne - piec</t>
+  </si>
+  <si>
+    <t>płyt G-K, scianki z płyt G-K</t>
+  </si>
+  <si>
+    <t>14 Roboty malarskie</t>
+  </si>
+  <si>
+    <t>15 Glazura</t>
+  </si>
+  <si>
+    <t>16 Parkiety, panele inne</t>
+  </si>
+  <si>
+    <t>17a Osprzet wodno-kanalizacyjny</t>
+  </si>
+  <si>
+    <t>17b Osprzet elektryczny</t>
+  </si>
+  <si>
+    <t>17c Grzejniki</t>
+  </si>
+  <si>
+    <t>18 Drzwi wewnetrzne</t>
+  </si>
+  <si>
+    <t>19 Meble wbudowane</t>
+  </si>
+  <si>
+    <t>VI Przyłacza</t>
+  </si>
+  <si>
+    <t>RAZEM (I - VI)</t>
+  </si>
+  <si>
+    <t>II STAN SUROWY ZADASZONY</t>
+  </si>
+  <si>
+    <t>12b Instalacje wewnetrzneelektryczna</t>
+  </si>
+  <si>
+    <t>12c Instalacje wewnetrzne- gazowa</t>
+  </si>
+  <si>
+    <t>12 f Instalacja WM</t>
+  </si>
+  <si>
+    <t>III STAN SUROWY ZAMKNIETY</t>
+  </si>
+  <si>
+    <t>13 Tynki wewnetrzne, okładziny z</t>
+  </si>
+  <si>
+    <t>20 Ocieplenie scian zewnetrznych, wykonczenie elewacji</t>
+  </si>
+  <si>
+    <t>IV STAN WYKONCZENIOWY</t>
+  </si>
+  <si>
+    <t>V WYKONCZENIE ZEWNETRZNE, Ogrodzenie, utwardzenie terenu</t>
+  </si>
+  <si>
+    <t>(dodać schody)</t>
+  </si>
+  <si>
+    <t>(rozbić na 12d)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$zł-415]_-;\-* #,##0.00\ [$zł-415]_-;_-* &quot;-&quot;??\ [$zł-415]_-;_-@_-"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,8 +673,17 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +738,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="41">
     <border>
@@ -1068,7 +1237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1414,15 +1583,135 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1441,131 +1730,33 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1839,19 +2030,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:G33" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:G33" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:G33">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="Warunek" dataDxfId="6"/>
-    <tableColumn id="2" name="N" dataDxfId="5"/>
-    <tableColumn id="3" name="S" dataDxfId="4"/>
-    <tableColumn id="4" name="M" dataDxfId="3"/>
-    <tableColumn id="5" name="TZI-Team" dataDxfId="2"/>
-    <tableColumn id="6" name="Ekipa5" dataDxfId="1"/>
-    <tableColumn id="7" name="Ekipa6" dataDxfId="0"/>
+    <tableColumn id="1" name="Warunek" dataDxfId="7"/>
+    <tableColumn id="2" name="N" dataDxfId="6"/>
+    <tableColumn id="3" name="S" dataDxfId="5"/>
+    <tableColumn id="4" name="M" dataDxfId="4"/>
+    <tableColumn id="5" name="TZI-Team" dataDxfId="3"/>
+    <tableColumn id="6" name="Ekipa5" dataDxfId="2"/>
+    <tableColumn id="7" name="Ekipa6" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2822,7 +3013,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="156" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -2832,7 +3023,7 @@
       <c r="D2" s="60"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="131"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="21" t="s">
         <v>49</v>
       </c>
@@ -2840,7 +3031,7 @@
       <c r="D3" s="61"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="131"/>
+      <c r="A4" s="157"/>
       <c r="B4" s="21" t="s">
         <v>50</v>
       </c>
@@ -2848,7 +3039,7 @@
       <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="131"/>
+      <c r="A5" s="157"/>
       <c r="B5" s="21" t="s">
         <v>51</v>
       </c>
@@ -2856,7 +3047,7 @@
       <c r="D5" s="62"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A6" s="132"/>
+      <c r="A6" s="158"/>
       <c r="B6" s="22" t="s">
         <v>52</v>
       </c>
@@ -2864,7 +3055,7 @@
       <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="156" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="92" t="s">
@@ -2874,7 +3065,7 @@
       <c r="D7" s="62"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="131"/>
+      <c r="A8" s="157"/>
       <c r="B8" s="21" t="s">
         <v>55</v>
       </c>
@@ -2882,7 +3073,7 @@
       <c r="D8" s="62"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A9" s="132"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="22" t="s">
         <v>56</v>
       </c>
@@ -2890,7 +3081,7 @@
       <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="130" t="s">
+      <c r="A10" s="156" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -2900,7 +3091,7 @@
       <c r="D10" s="62"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="131"/>
+      <c r="A11" s="157"/>
       <c r="B11" s="21" t="s">
         <v>59</v>
       </c>
@@ -2908,7 +3099,7 @@
       <c r="D11" s="62"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="131"/>
+      <c r="A12" s="157"/>
       <c r="B12" s="21" t="s">
         <v>60</v>
       </c>
@@ -2916,7 +3107,7 @@
       <c r="D12" s="62"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="131"/>
+      <c r="A13" s="157"/>
       <c r="B13" s="21" t="s">
         <v>61</v>
       </c>
@@ -2924,7 +3115,7 @@
       <c r="D13" s="62"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="131"/>
+      <c r="A14" s="157"/>
       <c r="B14" s="21" t="s">
         <v>52</v>
       </c>
@@ -2932,7 +3123,7 @@
       <c r="D14" s="62"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A15" s="132"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="22" t="s">
         <v>62</v>
       </c>
@@ -2950,7 +3141,7 @@
       <c r="D16" s="67"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="133" t="s">
+      <c r="A17" s="159" t="s">
         <v>64</v>
       </c>
       <c r="B17" s="93" t="s">
@@ -2960,7 +3151,7 @@
       <c r="D17" s="63"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="123"/>
+      <c r="A18" s="160"/>
       <c r="B18" s="88" t="s">
         <v>55</v>
       </c>
@@ -2968,7 +3159,7 @@
       <c r="D18" s="63"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="123"/>
+      <c r="A19" s="160"/>
       <c r="B19" s="88" t="s">
         <v>66</v>
       </c>
@@ -2976,7 +3167,7 @@
       <c r="D19" s="63"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="123"/>
+      <c r="A20" s="160"/>
       <c r="B20" s="88" t="s">
         <v>131</v>
       </c>
@@ -2984,7 +3175,7 @@
       <c r="D20" s="63"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A21" s="134"/>
+      <c r="A21" s="161"/>
       <c r="B21" s="89" t="s">
         <v>67</v>
       </c>
@@ -2992,7 +3183,7 @@
       <c r="D21" s="63"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="123" t="s">
+      <c r="A22" s="160" t="s">
         <v>68</v>
       </c>
       <c r="B22" s="94" t="s">
@@ -3002,7 +3193,7 @@
       <c r="D22" s="68"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="123"/>
+      <c r="A23" s="160"/>
       <c r="B23" s="88" t="s">
         <v>132</v>
       </c>
@@ -3010,7 +3201,7 @@
       <c r="D23" s="63"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="123"/>
+      <c r="A24" s="160"/>
       <c r="B24" s="88" t="s">
         <v>133</v>
       </c>
@@ -3018,7 +3209,7 @@
       <c r="D24" s="63"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="123"/>
+      <c r="A25" s="160"/>
       <c r="B25" s="88" t="s">
         <v>134</v>
       </c>
@@ -3026,7 +3217,7 @@
       <c r="D25" s="63"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="123"/>
+      <c r="A26" s="160"/>
       <c r="B26" s="88" t="s">
         <v>136</v>
       </c>
@@ -3034,7 +3225,7 @@
       <c r="D26" s="63"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A27" s="123"/>
+      <c r="A27" s="160"/>
       <c r="B27" s="88" t="s">
         <v>70</v>
       </c>
@@ -3042,7 +3233,7 @@
       <c r="D27" s="69"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="124" t="s">
+      <c r="A28" s="164" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="90" t="s">
@@ -3052,7 +3243,7 @@
       <c r="D28" s="64"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A29" s="125"/>
+      <c r="A29" s="165"/>
       <c r="B29" s="56" t="s">
         <v>86</v>
       </c>
@@ -3060,7 +3251,7 @@
       <c r="D29" s="64"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="126" t="s">
+      <c r="A30" s="166" t="s">
         <v>73</v>
       </c>
       <c r="B30" s="95" t="s">
@@ -3070,7 +3261,7 @@
       <c r="D30" s="70"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="126"/>
+      <c r="A31" s="166"/>
       <c r="B31" s="55" t="s">
         <v>75</v>
       </c>
@@ -3078,7 +3269,7 @@
       <c r="D31" s="64"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A32" s="125"/>
+      <c r="A32" s="165"/>
       <c r="B32" s="56" t="s">
         <v>87</v>
       </c>
@@ -3086,7 +3277,7 @@
       <c r="D32" s="71"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="127" t="s">
+      <c r="A33" s="167" t="s">
         <v>76</v>
       </c>
       <c r="B33" s="25" t="s">
@@ -3096,7 +3287,7 @@
       <c r="D33" s="65"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A34" s="128"/>
+      <c r="A34" s="168"/>
       <c r="B34" s="24" t="s">
         <v>67</v>
       </c>
@@ -3104,7 +3295,7 @@
       <c r="D34" s="65"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="127" t="s">
+      <c r="A35" s="167" t="s">
         <v>78</v>
       </c>
       <c r="B35" s="25" t="s">
@@ -3114,7 +3305,7 @@
       <c r="D35" s="83"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="129"/>
+      <c r="A36" s="169"/>
       <c r="B36" s="25" t="s">
         <v>80</v>
       </c>
@@ -3122,7 +3313,7 @@
       <c r="D36" s="65"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="129"/>
+      <c r="A37" s="169"/>
       <c r="B37" s="25" t="s">
         <v>88</v>
       </c>
@@ -3130,7 +3321,7 @@
       <c r="D37" s="65"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="129"/>
+      <c r="A38" s="169"/>
       <c r="B38" s="25" t="s">
         <v>81</v>
       </c>
@@ -3138,7 +3329,7 @@
       <c r="D38" s="65"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="129"/>
+      <c r="A39" s="169"/>
       <c r="B39" s="25" t="s">
         <v>82</v>
       </c>
@@ -3146,7 +3337,7 @@
       <c r="D39" s="65"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A40" s="128"/>
+      <c r="A40" s="168"/>
       <c r="B40" s="24" t="s">
         <v>83</v>
       </c>
@@ -3164,7 +3355,7 @@
       <c r="D41" s="66"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="121" t="s">
+      <c r="A42" s="162" t="s">
         <v>122</v>
       </c>
       <c r="B42" s="99" t="s">
@@ -3174,7 +3365,7 @@
       <c r="D42" s="102"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A43" s="122"/>
+      <c r="A43" s="163"/>
       <c r="B43" s="100" t="s">
         <v>131</v>
       </c>
@@ -3212,10 +3403,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3223,16 +3414,18 @@
     <col min="1" max="1" width="8.5703125" style="19" customWidth="1"/>
     <col min="2" max="2" width="38.140625" style="19" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="19" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15" style="19" customWidth="1"/>
+    <col min="7" max="7" width="10" style="19" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="19"/>
     <col min="9" max="9" width="11" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="19"/>
+    <col min="10" max="11" width="9.140625" style="19"/>
+    <col min="12" max="12" width="12.85546875" style="19" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:17" ht="31.5" customHeight="1" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>45</v>
       </c>
@@ -3267,8 +3460,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21.75" customHeight="1">
-      <c r="A2" s="130" t="s">
+    <row r="2" spans="1:17" ht="21.75" customHeight="1">
+      <c r="A2" s="156" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -3279,15 +3472,15 @@
       </c>
       <c r="D2" s="112"/>
       <c r="E2" s="116"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="149"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="135"/>
       <c r="I2" s="31"/>
       <c r="J2" s="73"/>
       <c r="K2" s="60"/>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="131"/>
+    <row r="3" spans="1:17">
+      <c r="A3" s="157"/>
       <c r="B3" s="21" t="s">
         <v>49</v>
       </c>
@@ -3296,15 +3489,15 @@
       </c>
       <c r="D3" s="109"/>
       <c r="E3" s="117"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="137"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="123"/>
       <c r="I3" s="32"/>
       <c r="J3" s="72"/>
       <c r="K3" s="61"/>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="131"/>
+    <row r="4" spans="1:17">
+      <c r="A4" s="157"/>
       <c r="B4" s="21" t="s">
         <v>50</v>
       </c>
@@ -3313,15 +3506,15 @@
       </c>
       <c r="D4" s="109"/>
       <c r="E4" s="110"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="138"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="124"/>
       <c r="I4" s="32"/>
       <c r="J4" s="72"/>
       <c r="K4" s="62"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="131"/>
+    <row r="5" spans="1:17">
+      <c r="A5" s="157"/>
       <c r="B5" s="21" t="s">
         <v>51</v>
       </c>
@@ -3330,15 +3523,15 @@
       </c>
       <c r="D5" s="109"/>
       <c r="E5" s="110"/>
-      <c r="F5" s="135"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="138"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="124"/>
       <c r="I5" s="32"/>
       <c r="J5" s="72"/>
       <c r="K5" s="62"/>
     </row>
-    <row r="6" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A6" s="132"/>
+    <row r="6" spans="1:17" ht="11.25" thickBot="1">
+      <c r="A6" s="158"/>
       <c r="B6" s="22" t="s">
         <v>52</v>
       </c>
@@ -3347,9 +3540,9 @@
       </c>
       <c r="D6" s="114"/>
       <c r="E6" s="115"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="141">
+      <c r="F6" s="125"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="127">
         <v>4800</v>
       </c>
       <c r="I6" s="33"/>
@@ -3358,8 +3551,8 @@
         <v>2612</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="130" t="s">
+    <row r="7" spans="1:17">
+      <c r="A7" s="156" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="92" t="s">
@@ -3370,15 +3563,15 @@
       </c>
       <c r="D7" s="109"/>
       <c r="E7" s="110"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="138"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="124"/>
       <c r="I7" s="34"/>
-      <c r="J7" s="151"/>
-      <c r="K7" s="153"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="131"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="139"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="157"/>
       <c r="B8" s="21" t="s">
         <v>55</v>
       </c>
@@ -3387,15 +3580,15 @@
       </c>
       <c r="D8" s="109"/>
       <c r="E8" s="110"/>
-      <c r="F8" s="142"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="138"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="124"/>
       <c r="I8" s="34"/>
-      <c r="J8" s="151"/>
-      <c r="K8" s="154"/>
-    </row>
-    <row r="9" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A9" s="132"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="140"/>
+    </row>
+    <row r="9" spans="1:17" ht="11.25" thickBot="1">
+      <c r="A9" s="158"/>
       <c r="B9" s="22" t="s">
         <v>56</v>
       </c>
@@ -3404,17 +3597,17 @@
       </c>
       <c r="D9" s="114"/>
       <c r="E9" s="115"/>
-      <c r="F9" s="143"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="141">
+      <c r="F9" s="129"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="127">
         <v>2700</v>
       </c>
       <c r="I9" s="35"/>
-      <c r="J9" s="152"/>
-      <c r="K9" s="154"/>
-    </row>
-    <row r="10" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A10" s="130" t="s">
+      <c r="J9" s="138"/>
+      <c r="K9" s="140"/>
+    </row>
+    <row r="10" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A10" s="156" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -3425,15 +3618,15 @@
       </c>
       <c r="D10" s="72"/>
       <c r="E10" s="62"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="138"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="124"/>
       <c r="I10" s="72"/>
-      <c r="J10" s="151"/>
-      <c r="K10" s="154"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="131"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="140"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="157"/>
       <c r="B11" s="21" t="s">
         <v>59</v>
       </c>
@@ -3442,15 +3635,15 @@
       </c>
       <c r="D11" s="72"/>
       <c r="E11" s="62"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="136"/>
-      <c r="H11" s="138"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="124"/>
       <c r="I11" s="72"/>
-      <c r="J11" s="151"/>
-      <c r="K11" s="154"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="131"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="140"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="157"/>
       <c r="B12" s="21" t="s">
         <v>60</v>
       </c>
@@ -3459,15 +3652,15 @@
       </c>
       <c r="D12" s="72"/>
       <c r="E12" s="62"/>
-      <c r="F12" s="136"/>
-      <c r="G12" s="136"/>
-      <c r="H12" s="138"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="124"/>
       <c r="I12" s="72"/>
-      <c r="J12" s="151"/>
-      <c r="K12" s="154"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="131"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="140"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="157"/>
       <c r="B13" s="21" t="s">
         <v>61</v>
       </c>
@@ -3476,15 +3669,15 @@
       </c>
       <c r="D13" s="72"/>
       <c r="E13" s="62"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="136"/>
-      <c r="H13" s="138"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="124"/>
       <c r="I13" s="72"/>
-      <c r="J13" s="151"/>
-      <c r="K13" s="154"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="131"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="140"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="157"/>
       <c r="B14" s="21" t="s">
         <v>52</v>
       </c>
@@ -3493,15 +3686,30 @@
       </c>
       <c r="D14" s="72"/>
       <c r="E14" s="62"/>
-      <c r="F14" s="136"/>
-      <c r="G14" s="136"/>
-      <c r="H14" s="138"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="124"/>
       <c r="I14" s="72"/>
-      <c r="J14" s="151"/>
-      <c r="K14" s="154"/>
-    </row>
-    <row r="15" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A15" s="132"/>
+      <c r="J14" s="137"/>
+      <c r="K14" s="140"/>
+      <c r="M14" s="170" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="171" t="s">
+        <v>144</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q14" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="11.25" thickBot="1">
+      <c r="A15" s="158"/>
       <c r="B15" s="22" t="s">
         <v>62</v>
       </c>
@@ -3512,19 +3720,23 @@
       <c r="E15" s="62">
         <v>12250</v>
       </c>
-      <c r="F15" s="136"/>
-      <c r="G15" s="136"/>
-      <c r="H15" s="138">
+      <c r="F15" s="122"/>
+      <c r="G15" s="122"/>
+      <c r="H15" s="124">
         <v>4100</v>
       </c>
       <c r="I15" s="72"/>
-      <c r="J15" s="151"/>
-      <c r="K15" s="154">
+      <c r="J15" s="137"/>
+      <c r="K15" s="140">
         <f>8600+4073</f>
         <v>12673</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="11.25" thickBot="1">
+      <c r="M15" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="N15" s="172"/>
+    </row>
+    <row r="16" spans="1:17" ht="11.25" thickBot="1">
       <c r="A16" s="22" t="s">
         <v>63</v>
       </c>
@@ -3538,30 +3750,70 @@
       <c r="E16" s="67">
         <v>750</v>
       </c>
-      <c r="F16" s="144"/>
-      <c r="G16" s="145"/>
-      <c r="H16" s="146">
+      <c r="F16" s="130"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="132">
         <v>900</v>
       </c>
       <c r="I16" s="91"/>
-      <c r="J16" s="156"/>
-      <c r="K16" s="155"/>
-    </row>
-    <row r="17" spans="1:11" ht="11.25" thickBot="1">
+      <c r="J16" s="142"/>
+      <c r="K16" s="141"/>
+      <c r="L16" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="M16" s="19">
+        <v>13000</v>
+      </c>
+      <c r="N16" s="172">
+        <v>16673</v>
+      </c>
+      <c r="O16" s="19">
+        <f>Q16*1.23</f>
+        <v>29889</v>
+      </c>
+      <c r="P16" s="19">
+        <f>Q16*1.08</f>
+        <v>26244</v>
+      </c>
+      <c r="Q16" s="19">
+        <v>24300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="11.25" thickBot="1">
       <c r="A17" s="105"/>
       <c r="B17" s="105"/>
-      <c r="C17" s="163"/>
+      <c r="C17" s="149"/>
       <c r="D17" s="44"/>
       <c r="E17" s="67"/>
-      <c r="F17" s="164"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="165"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="156"/>
-      <c r="K17" s="169"/>
-    </row>
-    <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="123" t="s">
+      <c r="F17" s="150"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="149"/>
+      <c r="J17" s="142"/>
+      <c r="K17" s="155"/>
+      <c r="L17" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="M17" s="19">
+        <v>15200</v>
+      </c>
+      <c r="N17" s="172">
+        <v>8850</v>
+      </c>
+      <c r="O17" s="19">
+        <f t="shared" ref="O17:O21" si="0">Q17*1.23</f>
+        <v>32349</v>
+      </c>
+      <c r="P17" s="19">
+        <f t="shared" ref="P17:P21" si="1">Q17*1.08</f>
+        <v>28404.000000000004</v>
+      </c>
+      <c r="Q17" s="19">
+        <v>26300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="10.5" customHeight="1">
+      <c r="A18" s="160" t="s">
         <v>64</v>
       </c>
       <c r="B18" s="94" t="s">
@@ -3576,11 +3828,31 @@
       <c r="G18" s="75"/>
       <c r="H18" s="63"/>
       <c r="I18" s="36"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="167"/>
-    </row>
-    <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="123"/>
+      <c r="J18" s="152"/>
+      <c r="K18" s="153"/>
+      <c r="L18" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="M18" s="19">
+        <v>10800</v>
+      </c>
+      <c r="N18" s="172">
+        <v>14000</v>
+      </c>
+      <c r="O18" s="19">
+        <f t="shared" si="0"/>
+        <v>24108</v>
+      </c>
+      <c r="P18" s="19">
+        <f t="shared" si="1"/>
+        <v>21168</v>
+      </c>
+      <c r="Q18" s="19">
+        <v>19600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="11.25" customHeight="1">
+      <c r="A19" s="160"/>
       <c r="B19" s="88" t="s">
         <v>55</v>
       </c>
@@ -3597,11 +3869,31 @@
       <c r="G19" s="75"/>
       <c r="H19" s="63"/>
       <c r="I19" s="36"/>
-      <c r="J19" s="166"/>
-      <c r="K19" s="168"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="123"/>
+      <c r="J19" s="152"/>
+      <c r="K19" s="154"/>
+      <c r="L19" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="M19" s="19">
+        <v>900</v>
+      </c>
+      <c r="N19" s="172">
+        <v>900</v>
+      </c>
+      <c r="O19" s="19">
+        <f t="shared" si="0"/>
+        <v>6150</v>
+      </c>
+      <c r="P19" s="19">
+        <f t="shared" si="1"/>
+        <v>5400</v>
+      </c>
+      <c r="Q19" s="19">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="160"/>
       <c r="B20" s="88" t="s">
         <v>66</v>
       </c>
@@ -3618,11 +3910,31 @@
       <c r="G20" s="75"/>
       <c r="H20" s="63"/>
       <c r="I20" s="36"/>
-      <c r="J20" s="166"/>
-      <c r="K20" s="168"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="123"/>
+      <c r="J20" s="152"/>
+      <c r="K20" s="154"/>
+      <c r="L20" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="M20" s="19">
+        <v>5000</v>
+      </c>
+      <c r="N20" s="172">
+        <v>4000</v>
+      </c>
+      <c r="O20" s="19">
+        <f t="shared" si="0"/>
+        <v>5535</v>
+      </c>
+      <c r="P20" s="19">
+        <f t="shared" si="1"/>
+        <v>4860</v>
+      </c>
+      <c r="Q20" s="19">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="160"/>
       <c r="B21" s="88" t="s">
         <v>131</v>
       </c>
@@ -3637,11 +3949,28 @@
       <c r="G21" s="75"/>
       <c r="H21" s="63"/>
       <c r="I21" s="36"/>
-      <c r="J21" s="166"/>
-      <c r="K21" s="168"/>
-    </row>
-    <row r="22" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A22" s="123"/>
+      <c r="J21" s="152"/>
+      <c r="K21" s="154"/>
+      <c r="L21" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="N21" s="172">
+        <v>2300</v>
+      </c>
+      <c r="O21" s="19">
+        <f t="shared" si="0"/>
+        <v>6826.5</v>
+      </c>
+      <c r="P21" s="19">
+        <f t="shared" si="1"/>
+        <v>5994</v>
+      </c>
+      <c r="Q21" s="19">
+        <v>5550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="11.25" thickBot="1">
+      <c r="A22" s="160"/>
       <c r="B22" s="88" t="s">
         <v>67</v>
       </c>
@@ -3660,11 +3989,27 @@
         <v>6700</v>
       </c>
       <c r="I22" s="36"/>
-      <c r="J22" s="166"/>
-      <c r="K22" s="168"/>
-    </row>
-    <row r="23" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A23" s="124" t="s">
+      <c r="J22" s="152"/>
+      <c r="K22" s="154"/>
+      <c r="M22" s="19">
+        <f>SUM(M16:M21)</f>
+        <v>44900</v>
+      </c>
+      <c r="N22" s="172">
+        <f>SUM(N16:N21)</f>
+        <v>46723</v>
+      </c>
+      <c r="O22" s="19">
+        <f>SUM(O16:O21)</f>
+        <v>104857.5</v>
+      </c>
+      <c r="P22" s="173">
+        <f>SUM(P16:P21)</f>
+        <v>92070</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="10.5" customHeight="1">
+      <c r="A23" s="164" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="90" t="s">
@@ -3681,11 +4026,12 @@
       <c r="G23" s="78"/>
       <c r="H23" s="70"/>
       <c r="I23" s="37"/>
-      <c r="J23" s="158"/>
-      <c r="K23" s="160"/>
-    </row>
-    <row r="24" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A24" s="125"/>
+      <c r="J23" s="144"/>
+      <c r="K23" s="146"/>
+      <c r="N23" s="172"/>
+    </row>
+    <row r="24" spans="1:17" ht="11.25" thickBot="1">
+      <c r="A24" s="165"/>
       <c r="B24" s="56" t="s">
         <v>86</v>
       </c>
@@ -3704,11 +4050,22 @@
         <v>2850</v>
       </c>
       <c r="I24" s="38"/>
-      <c r="J24" s="159"/>
-      <c r="K24" s="160"/>
-    </row>
-    <row r="25" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A25" s="126" t="s">
+      <c r="J24" s="145"/>
+      <c r="K24" s="146"/>
+      <c r="L24" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="M24" s="19">
+        <f>M22+O22</f>
+        <v>149757.5</v>
+      </c>
+      <c r="N24" s="173">
+        <f>N22+P22</f>
+        <v>138793</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="10.5" customHeight="1">
+      <c r="A25" s="166" t="s">
         <v>73</v>
       </c>
       <c r="B25" s="95" t="s">
@@ -3721,11 +4078,12 @@
       <c r="G25" s="77"/>
       <c r="H25" s="64"/>
       <c r="I25" s="39"/>
-      <c r="J25" s="157"/>
-      <c r="K25" s="160"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="126"/>
+      <c r="J25" s="143"/>
+      <c r="K25" s="146"/>
+      <c r="N25" s="172"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="166"/>
       <c r="B26" s="55" t="s">
         <v>75</v>
       </c>
@@ -3742,11 +4100,31 @@
       <c r="G26" s="77"/>
       <c r="H26" s="64"/>
       <c r="I26" s="39"/>
-      <c r="J26" s="157"/>
-      <c r="K26" s="160"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A27" s="125"/>
+      <c r="J26" s="143"/>
+      <c r="K26" s="146"/>
+      <c r="L26" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="M26" s="19">
+        <v>11200</v>
+      </c>
+      <c r="N26" s="172">
+        <v>20000</v>
+      </c>
+      <c r="O26" s="19">
+        <f t="shared" ref="O26" si="2">Q26*1.23</f>
+        <v>32349</v>
+      </c>
+      <c r="P26" s="19">
+        <f t="shared" ref="P26" si="3">Q26*1.08</f>
+        <v>28404.000000000004</v>
+      </c>
+      <c r="Q26" s="19">
+        <v>26300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A27" s="165"/>
       <c r="B27" s="56" t="s">
         <v>87</v>
       </c>
@@ -3765,14 +4143,14 @@
         <v>1900</v>
       </c>
       <c r="I27" s="38"/>
-      <c r="J27" s="159"/>
-      <c r="K27" s="161">
+      <c r="J27" s="145"/>
+      <c r="K27" s="147">
         <f>9775+2300</f>
         <v>12075</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="123" t="s">
+    <row r="28" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A28" s="160" t="s">
         <v>68</v>
       </c>
       <c r="B28" s="94" t="s">
@@ -3790,8 +4168,8 @@
       <c r="J28" s="76"/>
       <c r="K28" s="63"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="123"/>
+    <row r="29" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A29" s="160"/>
       <c r="B29" s="88" t="s">
         <v>132</v>
       </c>
@@ -3807,8 +4185,8 @@
       <c r="J29" s="75"/>
       <c r="K29" s="63"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="123"/>
+    <row r="30" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A30" s="160"/>
       <c r="B30" s="88" t="s">
         <v>133</v>
       </c>
@@ -3826,8 +4204,8 @@
       <c r="J30" s="75"/>
       <c r="K30" s="63"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="123"/>
+    <row r="31" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A31" s="160"/>
       <c r="B31" s="88" t="s">
         <v>134</v>
       </c>
@@ -3843,8 +4221,8 @@
       <c r="J31" s="75"/>
       <c r="K31" s="63"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="123"/>
+    <row r="32" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A32" s="160"/>
       <c r="B32" s="88" t="s">
         <v>136</v>
       </c>
@@ -3863,7 +4241,7 @@
       <c r="K32" s="63"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A33" s="123"/>
+      <c r="A33" s="160"/>
       <c r="B33" s="88" t="s">
         <v>70</v>
       </c>
@@ -3888,7 +4266,7 @@
       </c>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="127" t="s">
+      <c r="A34" s="167" t="s">
         <v>76</v>
       </c>
       <c r="B34" s="23" t="s">
@@ -3899,17 +4277,17 @@
       </c>
       <c r="D34" s="112"/>
       <c r="E34" s="113"/>
-      <c r="F34" s="162" t="s">
+      <c r="F34" s="148" t="s">
         <v>130</v>
       </c>
       <c r="G34" s="82"/>
       <c r="H34" s="83"/>
-      <c r="I34" s="162"/>
+      <c r="I34" s="148"/>
       <c r="J34" s="82"/>
       <c r="K34" s="83"/>
     </row>
     <row r="35" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A35" s="128"/>
+      <c r="A35" s="168"/>
       <c r="B35" s="24" t="s">
         <v>67</v>
       </c>
@@ -3932,7 +4310,7 @@
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="127" t="s">
+      <c r="A36" s="167" t="s">
         <v>78</v>
       </c>
       <c r="B36" s="25" t="s">
@@ -3953,7 +4331,7 @@
       <c r="K36" s="83"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="129"/>
+      <c r="A37" s="169"/>
       <c r="B37" s="25" t="s">
         <v>80</v>
       </c>
@@ -3972,7 +4350,7 @@
       <c r="K37" s="65"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="129"/>
+      <c r="A38" s="169"/>
       <c r="B38" s="25" t="s">
         <v>88</v>
       </c>
@@ -3991,7 +4369,7 @@
       <c r="K38" s="65"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="129"/>
+      <c r="A39" s="169"/>
       <c r="B39" s="25" t="s">
         <v>81</v>
       </c>
@@ -4010,7 +4388,7 @@
       <c r="K39" s="65"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="129"/>
+      <c r="A40" s="169"/>
       <c r="B40" s="25" t="s">
         <v>82</v>
       </c>
@@ -4029,7 +4407,7 @@
       <c r="K40" s="65"/>
     </row>
     <row r="41" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A41" s="128"/>
+      <c r="A41" s="168"/>
       <c r="B41" s="24" t="s">
         <v>83</v>
       </c>
@@ -4077,7 +4455,7 @@
       <c r="K42" s="66"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="121" t="s">
+      <c r="A43" s="162" t="s">
         <v>122</v>
       </c>
       <c r="B43" s="99" t="s">
@@ -4100,7 +4478,7 @@
       <c r="K43" s="102"/>
     </row>
     <row r="44" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A44" s="122"/>
+      <c r="A44" s="163"/>
       <c r="B44" s="100" t="s">
         <v>131</v>
       </c>
@@ -4171,13 +4549,13 @@
       </c>
       <c r="C47" s="49"/>
       <c r="D47" s="50"/>
-      <c r="E47" s="150">
+      <c r="E47" s="136">
         <f>E46+E45</f>
         <v>52386.13</v>
       </c>
       <c r="F47" s="49"/>
       <c r="G47" s="50"/>
-      <c r="H47" s="150">
+      <c r="H47" s="136">
         <f>H46+H45</f>
         <v>48546</v>
       </c>
@@ -4206,19 +4584,303 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="K15:N20">
+    <sortCondition sortBy="cellColor" ref="L20" dxfId="0"/>
+  </sortState>
   <mergeCells count="10">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="A28:A33"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9">
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="176">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="176">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="177">
+        <f>SUM(H1:H3)</f>
+        <v>39600</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H5" s="176">
+        <v>49000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H6" s="176">
+        <v>34000</v>
+      </c>
+      <c r="I6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="176">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="176">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H9" s="177">
+        <f>SUM(H5:H8)</f>
+        <v>127000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" s="176">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H11" s="176">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="176">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" s="176">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H14" s="176">
+        <v>26000</v>
+      </c>
+      <c r="I14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H15" s="176">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="174" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" s="176"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>170</v>
+      </c>
+      <c r="H17" s="176"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="176">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="H19" s="176">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>187</v>
+      </c>
+      <c r="H20" s="177">
+        <f>SUM(H10:H19)</f>
+        <v>162000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>188</v>
+      </c>
+      <c r="H21" s="176"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" t="s">
+        <v>172</v>
+      </c>
+      <c r="H22" s="176"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" t="s">
+        <v>173</v>
+      </c>
+      <c r="H23" s="176"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" t="s">
+        <v>174</v>
+      </c>
+      <c r="H24" s="176"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H25" s="176"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>176</v>
+      </c>
+      <c r="H26" s="176"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>177</v>
+      </c>
+      <c r="H27" s="176"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28" s="176"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" t="s">
+        <v>179</v>
+      </c>
+      <c r="H29" s="176"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
+        <v>180</v>
+      </c>
+      <c r="H30" s="176"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="175" t="s">
+        <v>189</v>
+      </c>
+      <c r="H31" s="176"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" t="s">
+        <v>190</v>
+      </c>
+      <c r="H32" s="176">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="H33" s="176"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" t="s">
+        <v>181</v>
+      </c>
+      <c r="H34" s="176"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" s="176"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="H36" s="177">
+        <f>SUM(H32,H20,H9,H4)</f>
+        <v>468600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>